<commit_message>
work on EDUCATION death data, and file name clean up
</commit_message>
<xml_diff>
--- a/myUpstream/upstreamInfo/death.File.Vars.xlsx
+++ b/myUpstream/upstreamInfo/death.File.Vars.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0.CBD\myUpstream\upstreamInfo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="12345"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="varNameInfo" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -317,7 +312,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -723,7 +718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -734,7 +729,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update CCB data using new condition list
</commit_message>
<xml_diff>
--- a/myUpstream/upstreamInfo/death.File.Vars.xlsx
+++ b/myUpstream/upstreamInfo/death.File.Vars.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myUpstream\upstreamInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7004AB-EC0A-472A-A5F3-877D89D57504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB3280F-3F05-4C62-9A93-B3BB563A1636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7695" yWindow="4290" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variableNames" sheetId="1" r:id="rId1"/>
     <sheet name="varNameInfo" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="128">
   <si>
     <t>F12</t>
   </si>
@@ -567,6 +567,12 @@
   </si>
   <si>
     <t>countyFIPS_backup</t>
+  </si>
+  <si>
+    <t>birthCountry</t>
+  </si>
+  <si>
+    <t>F29</t>
   </si>
 </sst>
 </file>
@@ -1058,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,448 +1179,459 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>70</v>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>243</v>
-      </c>
-      <c r="F10">
-        <v>247</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>243</v>
-      </c>
-      <c r="I10">
-        <v>247</v>
+      <c r="C10" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>181</v>
+        <v>243</v>
       </c>
       <c r="F11">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11" s="14">
-        <v>156</v>
-      </c>
-      <c r="I11" s="14">
-        <v>156</v>
+      <c r="H11">
+        <v>243</v>
+      </c>
+      <c r="I11">
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12">
+        <v>181</v>
+      </c>
+      <c r="F12">
+        <v>182</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14">
         <v>156</v>
       </c>
-      <c r="F12">
-        <v>157</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="14">
-        <v>157</v>
-      </c>
       <c r="I12" s="14">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="F13">
-        <v>131</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+        <v>157</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14">
+        <v>157</v>
+      </c>
+      <c r="I13" s="14">
+        <v>158</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>126</v>
+      </c>
+      <c r="F14">
+        <v>131</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>77</v>
-      </c>
-      <c r="F15">
-        <v>77</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>77</v>
-      </c>
-      <c r="I15">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I16">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F17">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="I17">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>120</v>
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>66</v>
+      </c>
+      <c r="F18">
+        <v>66</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>66</v>
+      </c>
+      <c r="I18">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>242</v>
-      </c>
-      <c r="F21">
-        <v>242</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>242</v>
-      </c>
-      <c r="I21">
-        <v>242</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="F22">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22">
-        <v>174</v>
+        <v>242</v>
       </c>
       <c r="I22">
-        <v>174</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>123</v>
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>174</v>
+      </c>
+      <c r="F23">
+        <v>174</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>174</v>
+      </c>
+      <c r="I23">
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>201</v>
-      </c>
-      <c r="F24">
-        <v>201</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>201</v>
-      </c>
-      <c r="I24">
-        <v>201</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="F25">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="I25">
-        <v>165</v>
+        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>103</v>
-      </c>
-      <c r="B26" t="s">
-        <v>105</v>
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>105</v>
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>161</v>
+      </c>
+      <c r="F26">
+        <v>165</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26">
-        <v>7</v>
+        <v>161</v>
       </c>
       <c r="I26">
-        <v>12</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
-        <v>172</v>
+        <v>7</v>
       </c>
       <c r="I27">
-        <v>173</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>172</v>
+      </c>
+      <c r="I28">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>115</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>